<commit_message>
added post drs work inc grid
</commit_message>
<xml_diff>
--- a/Results/Training Record.xlsx
+++ b/Results/Training Record.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/djw1g12/mydocuments/Demonstrating/Chomp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/djw1g12/mydocuments/Demonstrating/Chomp/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{524B71C5-E3F9-F84F-8611-B7FF07FD9ADF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AAD857A2-1693-344E-B18C-02C40DA1649E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="27320" windowHeight="14820" xr2:uid="{9759C974-99C7-644E-B88E-259FDE16B5DB}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27320" windowHeight="14820" activeTab="1" xr2:uid="{9759C974-99C7-644E-B88E-259FDE16B5DB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="After 76 Games" sheetId="1" r:id="rId1"/>
+    <sheet name="After 98 Games" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t xml:space="preserve">Box </t>
   </si>
@@ -494,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3E01A9-281A-2C4F-BC9E-5180F9ED5D0B}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -1168,4 +1169,663 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ADEDA7-472E-9A4C-95F8-D7BD9289C85E}">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
+    <col min="7" max="7" width="10.83203125" style="7"/>
+    <col min="8" max="8" width="10.83203125" style="8"/>
+    <col min="9" max="9" width="10.83203125" style="9"/>
+    <col min="10" max="10" width="10.83203125" style="10"/>
+    <col min="11" max="11" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>4</v>
+      </c>
+      <c r="H14" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="E15" s="5">
+        <v>28</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2</v>
+      </c>
+      <c r="I16" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>2</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6">
+        <v>2</v>
+      </c>
+      <c r="I20" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>2</v>
+      </c>
+      <c r="I21" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>2</v>
+      </c>
+      <c r="I22" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>6</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>2</v>
+      </c>
+      <c r="I23" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="C24" s="3">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>2</v>
+      </c>
+      <c r="F24" s="6">
+        <v>2</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
+      <c r="H24" s="8">
+        <v>2</v>
+      </c>
+      <c r="I24" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="I25" s="9">
+        <v>2</v>
+      </c>
+      <c r="J25" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="5">
+        <v>2</v>
+      </c>
+      <c r="F26" s="6">
+        <v>4</v>
+      </c>
+      <c r="I26" s="9">
+        <v>3</v>
+      </c>
+      <c r="J26" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
+        <v>4</v>
+      </c>
+      <c r="D27" s="4">
+        <v>3</v>
+      </c>
+      <c r="F27" s="6">
+        <v>11</v>
+      </c>
+      <c r="I27" s="9">
+        <v>8</v>
+      </c>
+      <c r="J27" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5">
+        <v>2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>4</v>
+      </c>
+      <c r="G28" s="7">
+        <v>4</v>
+      </c>
+      <c r="I28" s="9">
+        <v>2</v>
+      </c>
+      <c r="J28" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9">
+        <v>2</v>
+      </c>
+      <c r="J29" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>5</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5">
+        <v>5</v>
+      </c>
+      <c r="F30" s="6">
+        <v>4</v>
+      </c>
+      <c r="G30" s="7">
+        <v>5</v>
+      </c>
+      <c r="H30" s="8">
+        <v>5</v>
+      </c>
+      <c r="I30" s="9">
+        <v>3</v>
+      </c>
+      <c r="J30" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>2</v>
+      </c>
+      <c r="F31" s="6">
+        <v>12</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1</v>
+      </c>
+      <c r="I31" s="9">
+        <v>6</v>
+      </c>
+      <c r="J31" s="10">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3">
+        <v>8</v>
+      </c>
+      <c r="E32" s="5">
+        <v>3</v>
+      </c>
+      <c r="F32" s="6">
+        <v>3</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9">
+        <v>2</v>
+      </c>
+      <c r="J32" s="10">
+        <v>2</v>
+      </c>
+      <c r="K32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5</v>
+      </c>
+      <c r="E33" s="5">
+        <v>3</v>
+      </c>
+      <c r="F33" s="6">
+        <v>2</v>
+      </c>
+      <c r="G33" s="7">
+        <v>3</v>
+      </c>
+      <c r="H33" s="8">
+        <v>3</v>
+      </c>
+      <c r="I33" s="9">
+        <v>3</v>
+      </c>
+      <c r="J33" s="10">
+        <v>5</v>
+      </c>
+      <c r="K33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="C34" s="3">
+        <v>19</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2</v>
+      </c>
+      <c r="F34" s="6">
+        <v>15</v>
+      </c>
+      <c r="G34" s="7">
+        <v>10</v>
+      </c>
+      <c r="H34" s="8">
+        <v>21</v>
+      </c>
+      <c r="I34" s="9">
+        <v>5</v>
+      </c>
+      <c r="J34" s="10">
+        <v>12</v>
+      </c>
+      <c r="K34" s="1">
+        <v>4</v>
+      </c>
+      <c r="L34" s="11">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added comments, reflection and best fist fill graph python things
</commit_message>
<xml_diff>
--- a/Results/Training Record.xlsx
+++ b/Results/Training Record.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/djw1g12/mydocuments/Demonstrating/Chomp/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AAD857A2-1693-344E-B18C-02C40DA1649E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{45925D11-ED6C-E049-BD26-870226E2FBED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="27320" windowHeight="14820" activeTab="1" xr2:uid="{9759C974-99C7-644E-B88E-259FDE16B5DB}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="13660" windowHeight="14820" activeTab="2" xr2:uid="{9759C974-99C7-644E-B88E-259FDE16B5DB}"/>
   </bookViews>
   <sheets>
     <sheet name="After 76 Games" sheetId="1" r:id="rId1"/>
     <sheet name="After 98 Games" sheetId="2" r:id="rId2"/>
+    <sheet name="After csf 143 games" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
     <t xml:space="preserve">Box </t>
   </si>
@@ -1175,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ADEDA7-472E-9A4C-95F8-D7BD9289C85E}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1828,4 +1829,641 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3603D8BA-64D9-814F-8E88-39A2918154CD}">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="10.83203125" style="5"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
+    <col min="7" max="7" width="10.83203125" style="7"/>
+    <col min="8" max="8" width="10.83203125" style="8"/>
+    <col min="9" max="9" width="10.83203125" style="9"/>
+    <col min="10" max="10" width="10.83203125" style="10"/>
+    <col min="11" max="11" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>2</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3</v>
+      </c>
+      <c r="H14" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="E15" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="I17" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4">
+        <v>19</v>
+      </c>
+      <c r="I18" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="I19" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3</v>
+      </c>
+      <c r="F21" s="6">
+        <v>6</v>
+      </c>
+      <c r="I21" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>2</v>
+      </c>
+      <c r="I23" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5">
+        <v>4</v>
+      </c>
+      <c r="F24" s="6">
+        <v>4</v>
+      </c>
+      <c r="G24" s="7">
+        <v>3</v>
+      </c>
+      <c r="H24" s="8">
+        <v>2</v>
+      </c>
+      <c r="I24" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="J25" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
+        <v>10</v>
+      </c>
+      <c r="I26" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="C27" s="3">
+        <v>11</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>18</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
+        <v>2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>4</v>
+      </c>
+      <c r="G28" s="7">
+        <v>2</v>
+      </c>
+      <c r="I28" s="9">
+        <v>4</v>
+      </c>
+      <c r="J28" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>2</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+      <c r="G29" s="7">
+        <v>2</v>
+      </c>
+      <c r="I29" s="9">
+        <v>4</v>
+      </c>
+      <c r="J29" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
+        <v>4</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3</v>
+      </c>
+      <c r="F30" s="6">
+        <v>2</v>
+      </c>
+      <c r="G30" s="7">
+        <v>3</v>
+      </c>
+      <c r="H30" s="8">
+        <v>5</v>
+      </c>
+      <c r="I30" s="9">
+        <v>8</v>
+      </c>
+      <c r="J30" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="6">
+        <v>4</v>
+      </c>
+      <c r="G31" s="7">
+        <v>11</v>
+      </c>
+      <c r="I31" s="9">
+        <v>7</v>
+      </c>
+      <c r="J31" s="10">
+        <v>4</v>
+      </c>
+      <c r="K31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>4</v>
+      </c>
+      <c r="E32" s="5">
+        <v>1</v>
+      </c>
+      <c r="F32" s="6">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7">
+        <v>5</v>
+      </c>
+      <c r="I32" s="9">
+        <v>2</v>
+      </c>
+      <c r="J32" s="10">
+        <v>2</v>
+      </c>
+      <c r="K32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1</v>
+      </c>
+      <c r="F33" s="6">
+        <v>7</v>
+      </c>
+      <c r="G33" s="7">
+        <v>18</v>
+      </c>
+      <c r="H33" s="8">
+        <v>4</v>
+      </c>
+      <c r="J33" s="10">
+        <v>3</v>
+      </c>
+      <c r="K33" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="C34" s="3">
+        <v>31</v>
+      </c>
+      <c r="D34" s="4">
+        <v>11</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="8">
+        <v>19</v>
+      </c>
+      <c r="I34" s="9">
+        <v>3</v>
+      </c>
+      <c r="J34" s="10">
+        <v>2</v>
+      </c>
+      <c r="K34" s="1">
+        <v>13</v>
+      </c>
+      <c r="L34" s="11">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Chomp Paper and performance chart
</commit_message>
<xml_diff>
--- a/Results/Training Record.xlsx
+++ b/Results/Training Record.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filestore.soton.ac.uk\users\djw1g12\mydocuments\Demonstrating\Chomp\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3E9137-8733-48BF-8F74-853ACADC2BF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="13665" windowHeight="14820" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="13665" windowHeight="14820" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load" sheetId="6" r:id="rId1"/>
@@ -17,18 +18,24 @@
     <sheet name="After 98 Games" sheetId="2" r:id="rId3"/>
     <sheet name="After csf 143 games" sheetId="3" r:id="rId4"/>
     <sheet name="after SED19 86 games" sheetId="4" r:id="rId5"/>
+    <sheet name="after WSC + SiP 75 games " sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="27">
   <si>
     <t xml:space="preserve">Box </t>
   </si>
@@ -107,11 +114,14 @@
   <si>
     <t>Correct?</t>
   </si>
+  <si>
+    <t>BLUE/BLACK/ORANGE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -578,7 +588,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -1461,7 +1471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -2841,7 +2851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -4201,10 +4211,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
@@ -5539,11 +5549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -6879,4 +6889,1562 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF734A88-B3C7-4F82-BA32-5D5C190048BF}">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="11"/>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <f>MAX(B2:L2)</f>
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <f>MATCH(O2,B2:L2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>INDEX($B$1:$L$1,P2)</f>
+        <v>RED</v>
+      </c>
+      <c r="R2" t="b">
+        <f>ISNUMBER(SEARCH(Q2,M2))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="11"/>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O34" si="0">MAX(B3:L3)</f>
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P34" si="1">MATCH(O3,B3:L3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q34" si="2">INDEX($B$1:$L$1,P3)</f>
+        <v>RED</v>
+      </c>
+      <c r="R3" t="b">
+        <f t="shared" ref="R3:R34" si="3">ISNUMBER(SEARCH(Q3,M3))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="11"/>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <f>MAX(B4:L4)</f>
+        <v>19</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="2"/>
+        <v>RED</v>
+      </c>
+      <c r="R4" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="11"/>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="2"/>
+        <v>GREEN</v>
+      </c>
+      <c r="R5" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="11"/>
+      <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="2"/>
+        <v>GREEN</v>
+      </c>
+      <c r="R6" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="11"/>
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q7" t="str">
+        <f>INDEX($B$1:$L$1,P7)</f>
+        <v>RED</v>
+      </c>
+      <c r="R7" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="11"/>
+      <c r="M8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="2"/>
+        <v>ORANGE</v>
+      </c>
+      <c r="R8" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6">
+        <v>15</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="11"/>
+      <c r="M9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="2"/>
+        <v>BLUE</v>
+      </c>
+      <c r="R9" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="11"/>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="2"/>
+        <v>ORANGE</v>
+      </c>
+      <c r="R10" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="11"/>
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="2"/>
+        <v>YELLOW</v>
+      </c>
+      <c r="R11" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="11"/>
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="2"/>
+        <v>PURPLE</v>
+      </c>
+      <c r="R12" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>4</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="11"/>
+      <c r="M13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="2"/>
+        <v>BLUE</v>
+      </c>
+      <c r="R13" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>10</v>
+      </c>
+      <c r="H14" s="8">
+        <v>4</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="11"/>
+      <c r="M14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="2"/>
+        <v>PURPLE</v>
+      </c>
+      <c r="R14" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5">
+        <v>4</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="11"/>
+      <c r="M15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="2"/>
+        <v>GREEN</v>
+      </c>
+      <c r="R15" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9">
+        <v>8</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="11"/>
+      <c r="M16" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="2"/>
+        <v>BLACK</v>
+      </c>
+      <c r="R16" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9">
+        <v>4</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="11"/>
+      <c r="M17" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="2"/>
+        <v>BLACK</v>
+      </c>
+      <c r="R17" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="11"/>
+      <c r="M18" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="2"/>
+        <v>ORANGE</v>
+      </c>
+      <c r="R18" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>4</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="9">
+        <v>3</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="11"/>
+      <c r="M19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="2"/>
+        <v>BLUE</v>
+      </c>
+      <c r="R19" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9">
+        <v>2</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="11"/>
+      <c r="M20" t="s">
+        <v>26</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="2"/>
+        <v>GREEN</v>
+      </c>
+      <c r="R20" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6">
+        <v>2</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9">
+        <v>2</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="11"/>
+      <c r="M21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="2"/>
+        <v>RED</v>
+      </c>
+      <c r="R21" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>6</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9">
+        <v>3</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="11"/>
+      <c r="M22" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="2"/>
+        <v>PURPLE</v>
+      </c>
+      <c r="R22" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>2</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9">
+        <v>2</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="11"/>
+      <c r="M23" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="2"/>
+        <v>RED</v>
+      </c>
+      <c r="R23" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6">
+        <v>4</v>
+      </c>
+      <c r="G24" s="7">
+        <v>2</v>
+      </c>
+      <c r="H24" s="8">
+        <v>2</v>
+      </c>
+      <c r="I24" s="9">
+        <v>2</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="11"/>
+      <c r="M24" t="s">
+        <v>3</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="2"/>
+        <v>BLUE</v>
+      </c>
+      <c r="R24" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6">
+        <v>4</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10">
+        <v>15</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="11"/>
+      <c r="M25" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="2"/>
+        <v>GREY</v>
+      </c>
+      <c r="R25" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5">
+        <v>2</v>
+      </c>
+      <c r="F26" s="6">
+        <v>2</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10">
+        <v>4</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="11"/>
+      <c r="M26" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="2"/>
+        <v>GREY</v>
+      </c>
+      <c r="R26" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>4</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>2</v>
+      </c>
+      <c r="F27" s="6">
+        <v>2</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="9">
+        <v>10</v>
+      </c>
+      <c r="J27" s="10">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="11"/>
+      <c r="M27" t="s">
+        <v>10</v>
+      </c>
+      <c r="N27" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="2"/>
+        <v>BLACK</v>
+      </c>
+      <c r="R27" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5">
+        <v>2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>2</v>
+      </c>
+      <c r="G28" s="7">
+        <v>2</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="9">
+        <v>2</v>
+      </c>
+      <c r="J28" s="10">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="11"/>
+      <c r="M28" t="s">
+        <v>13</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="2"/>
+        <v>RED</v>
+      </c>
+      <c r="R28" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+      <c r="G29" s="7">
+        <v>2</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="9">
+        <v>2</v>
+      </c>
+      <c r="J29" s="10">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="11"/>
+      <c r="M29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="2"/>
+        <v>YELLOW</v>
+      </c>
+      <c r="R29" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3</v>
+      </c>
+      <c r="E30" s="5">
+        <v>1</v>
+      </c>
+      <c r="F30" s="6">
+        <v>3</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="8">
+        <v>3</v>
+      </c>
+      <c r="I30" s="9">
+        <v>5</v>
+      </c>
+      <c r="J30" s="10">
+        <v>5</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="11"/>
+      <c r="M30" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="2"/>
+        <v>BLACK</v>
+      </c>
+      <c r="R30" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="6">
+        <v>4</v>
+      </c>
+      <c r="G31" s="7">
+        <v>2</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="9">
+        <v>2</v>
+      </c>
+      <c r="J31" s="10">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1">
+        <v>4</v>
+      </c>
+      <c r="L31" s="11"/>
+      <c r="M31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="2"/>
+        <v>BLUE</v>
+      </c>
+      <c r="R31" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3</v>
+      </c>
+      <c r="E32" s="5">
+        <v>2</v>
+      </c>
+      <c r="F32" s="6">
+        <v>4</v>
+      </c>
+      <c r="G32" s="7">
+        <v>3</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9">
+        <v>4</v>
+      </c>
+      <c r="J32" s="10">
+        <v>3</v>
+      </c>
+      <c r="K32" s="1">
+        <v>5</v>
+      </c>
+      <c r="L32" s="11"/>
+      <c r="M32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="2"/>
+        <v>WHITE</v>
+      </c>
+      <c r="R32" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4</v>
+      </c>
+      <c r="D33" s="4">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1</v>
+      </c>
+      <c r="F33" s="6">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7">
+        <v>6</v>
+      </c>
+      <c r="H33" s="8">
+        <v>2</v>
+      </c>
+      <c r="I33" s="9">
+        <v>1</v>
+      </c>
+      <c r="J33" s="10">
+        <v>3</v>
+      </c>
+      <c r="K33" s="1">
+        <v>3</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" t="s">
+        <v>11</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="2"/>
+        <v>PURPLE</v>
+      </c>
+      <c r="R33" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3">
+        <v>22</v>
+      </c>
+      <c r="D34" s="4">
+        <v>5</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6">
+        <v>10</v>
+      </c>
+      <c r="G34" s="7">
+        <v>7</v>
+      </c>
+      <c r="H34" s="8"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="10">
+        <v>6</v>
+      </c>
+      <c r="K34" s="1">
+        <v>13</v>
+      </c>
+      <c r="L34" s="11">
+        <v>13</v>
+      </c>
+      <c r="M34" t="s">
+        <v>11</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="2"/>
+        <v>ORANGE</v>
+      </c>
+      <c r="R34" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>